<commit_message>
Tidy up simulation set ups and obs data.  Add phenology overwrites
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/data/DookieWWHI2024.xlsx
+++ b/Tests/Validation/Wheat/data/DookieWWHI2024.xlsx
@@ -67,52 +67,52 @@
     <t>Clock.Today</t>
   </si>
   <si>
-    <t>DookieWWHI2024CvGregory</t>
+    <t>DookieWWHI2024CvGregorySow14-May</t>
   </si>
   <si>
-    <t>DookieWWHI2024CvIllabo</t>
+    <t>DookieWWHI2024CvIllaboSow17-Apr</t>
   </si>
   <si>
-    <t>DookieWWHI2024CvJanz</t>
+    <t>DookieWWHI2024CvJanzSow14-May</t>
   </si>
   <si>
-    <t>DookieWWHI2024CvKittyhawk</t>
+    <t>DookieWWHI2024CvKittyhawkSow17-Apr</t>
   </si>
   <si>
-    <t>DookieWWHI2024CvMace</t>
+    <t>DookieWWHI2024CvMaceSow14-May</t>
   </si>
   <si>
-    <t>DookieWWHI2024CvMeering</t>
+    <t>DookieWWHI2024CvMeeringSow14-May</t>
   </si>
   <si>
-    <t>DookieWWHI2024CvMowhawk</t>
+    <t>DookieWWHI2024CvMowhawkSow17-Apr</t>
   </si>
   <si>
-    <t>DookieWWHI2024CvOsprey</t>
+    <t>DookieWWHI2024CvOspreySow17-Apr</t>
   </si>
   <si>
-    <t>DookieWWHI2024CvRosella</t>
+    <t>DookieWWHI2024CvRosellaSow17-Apr</t>
   </si>
   <si>
-    <t>DookieWWHI2024CvScepter</t>
+    <t>DookieWWHI2024CvScepterSow14-May</t>
   </si>
   <si>
-    <t>DookieWWHI2024CvSunmaster</t>
+    <t>DookieWWHI2024CvSunmasterSow14-May</t>
   </si>
   <si>
-    <t>DookieWWHI2024CvWedgetail</t>
+    <t>DookieWWHI2024CvWedgetailSow17-Apr</t>
   </si>
   <si>
-    <t>DookieWWHI2024CvWhistler</t>
+    <t>DookieWWHI2024CvWhistlerSow17-Apr</t>
   </si>
   <si>
-    <t>DookieWWHI2024CvWyalkatchem</t>
+    <t>DookieWWHI2024CvWyalkatchemSow14-May</t>
   </si>
   <si>
-    <t>DookieWWHI2024CvWylah</t>
+    <t>DookieWWHI2024CvWylahSow17-Apr</t>
   </si>
   <si>
-    <t>DookieWWHI2024CvYitpi</t>
+    <t>DookieWWHI2024CvYitpiSow14-May</t>
   </si>
 </sst>
 </file>
@@ -3227,7 +3227,7 @@
         <v>45559</v>
       </c>
       <c r="E246">
-        <v>14</v>
+        <v>13.25</v>
       </c>
     </row>
     <row r="247" spans="1:5">
@@ -3920,7 +3920,7 @@
         <v>45559</v>
       </c>
       <c r="E309">
-        <v>11</v>
+        <v>10.08333333333333</v>
       </c>
     </row>
     <row r="310" spans="1:5">
@@ -4239,7 +4239,7 @@
         <v>45559</v>
       </c>
       <c r="E338">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="339" spans="1:5">
@@ -4360,7 +4360,7 @@
         <v>45559</v>
       </c>
       <c r="E349">
-        <v>14</v>
+        <v>13.41666666666667</v>
       </c>
     </row>
     <row r="350" spans="1:5">
@@ -4924,7 +4924,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="401" spans="1:13">
+    <row r="401" spans="1:14">
       <c r="A401" s="1" t="s">
         <v>28</v>
       </c>
@@ -4935,7 +4935,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="402" spans="1:13">
+    <row r="402" spans="1:14">
       <c r="A402" s="1" t="s">
         <v>29</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="403" spans="1:13">
+    <row r="403" spans="1:14">
       <c r="A403" s="1" t="s">
         <v>30</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="404" spans="1:13">
+    <row r="404" spans="1:14">
       <c r="A404" s="1" t="s">
         <v>31</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="405" spans="1:13">
+    <row r="405" spans="1:14">
       <c r="A405" s="1" t="s">
         <v>32</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="406" spans="1:13">
+    <row r="406" spans="1:14">
       <c r="A406" s="1" t="s">
         <v>17</v>
       </c>
@@ -5010,8 +5010,11 @@
       <c r="M406">
         <v>544.5363368358067</v>
       </c>
-    </row>
-    <row r="407" spans="1:13">
+      <c r="N406">
+        <v>25.49066620045073</v>
+      </c>
+    </row>
+    <row r="407" spans="1:14">
       <c r="A407" s="1" t="s">
         <v>18</v>
       </c>
@@ -5042,8 +5045,11 @@
       <c r="M407">
         <v>745.4328028113457</v>
       </c>
-    </row>
-    <row r="408" spans="1:13">
+      <c r="N407">
+        <v>54.59546454941584</v>
+      </c>
+    </row>
+    <row r="408" spans="1:14">
       <c r="A408" s="1" t="s">
         <v>19</v>
       </c>
@@ -5074,8 +5080,11 @@
       <c r="M408">
         <v>552.1677637429648</v>
       </c>
-    </row>
-    <row r="409" spans="1:13">
+      <c r="N408">
+        <v>47.85054243215831</v>
+      </c>
+    </row>
+    <row r="409" spans="1:14">
       <c r="A409" s="1" t="s">
         <v>20</v>
       </c>
@@ -5106,8 +5115,11 @@
       <c r="M409">
         <v>672.9144861778489</v>
       </c>
-    </row>
-    <row r="410" spans="1:13">
+      <c r="N409">
+        <v>38.48922770060565</v>
+      </c>
+    </row>
+    <row r="410" spans="1:14">
       <c r="A410" s="1" t="s">
         <v>21</v>
       </c>
@@ -5138,8 +5150,11 @@
       <c r="M410">
         <v>484.7463144090221</v>
       </c>
-    </row>
-    <row r="411" spans="1:13">
+      <c r="N410">
+        <v>45.24337954959397</v>
+      </c>
+    </row>
+    <row r="411" spans="1:14">
       <c r="A411" s="1" t="s">
         <v>22</v>
       </c>
@@ -5170,8 +5185,11 @@
       <c r="M411">
         <v>543.7759863136012</v>
       </c>
-    </row>
-    <row r="412" spans="1:13">
+      <c r="N411">
+        <v>31.27599153514972</v>
+      </c>
+    </row>
+    <row r="412" spans="1:14">
       <c r="A412" s="1" t="s">
         <v>23</v>
       </c>
@@ -5202,8 +5220,11 @@
       <c r="M412">
         <v>643.0186602716327</v>
       </c>
-    </row>
-    <row r="413" spans="1:13">
+      <c r="N412">
+        <v>33.02415867481317</v>
+      </c>
+    </row>
+    <row r="413" spans="1:14">
       <c r="A413" s="1" t="s">
         <v>24</v>
       </c>
@@ -5234,8 +5255,11 @@
       <c r="M413">
         <v>617.2087877474071</v>
       </c>
-    </row>
-    <row r="414" spans="1:13">
+      <c r="N413">
+        <v>50.32241439318124</v>
+      </c>
+    </row>
+    <row r="414" spans="1:14">
       <c r="A414" s="1" t="s">
         <v>25</v>
       </c>
@@ -5266,8 +5290,11 @@
       <c r="M414">
         <v>696.4729968087037</v>
       </c>
-    </row>
-    <row r="415" spans="1:13">
+      <c r="N414">
+        <v>46.66026104325931</v>
+      </c>
+    </row>
+    <row r="415" spans="1:14">
       <c r="A415" s="1" t="s">
         <v>26</v>
       </c>
@@ -5298,8 +5325,11 @@
       <c r="M415">
         <v>545.0616366207109</v>
       </c>
-    </row>
-    <row r="416" spans="1:13">
+      <c r="N415">
+        <v>46.63882578677414</v>
+      </c>
+    </row>
+    <row r="416" spans="1:14">
       <c r="A416" s="1" t="s">
         <v>27</v>
       </c>
@@ -5329,6 +5359,9 @@
       </c>
       <c r="M416">
         <v>590.789907762931</v>
+      </c>
+      <c r="N416">
+        <v>22.59565709409236</v>
       </c>
     </row>
     <row r="417" spans="1:14">
@@ -5362,6 +5395,9 @@
       <c r="M417">
         <v>610.8927840958972</v>
       </c>
+      <c r="N417">
+        <v>30.2768196798471</v>
+      </c>
     </row>
     <row r="418" spans="1:14">
       <c r="A418" s="1" t="s">
@@ -5394,6 +5430,9 @@
       <c r="M418">
         <v>697.5701051121385</v>
       </c>
+      <c r="N418">
+        <v>37.44292329824293</v>
+      </c>
     </row>
     <row r="419" spans="1:14">
       <c r="A419" s="1" t="s">
@@ -5426,6 +5465,9 @@
       <c r="M419">
         <v>625.3145020267606</v>
       </c>
+      <c r="N419">
+        <v>46.87923815117863</v>
+      </c>
     </row>
     <row r="420" spans="1:14">
       <c r="A420" s="1" t="s">
@@ -5458,6 +5500,9 @@
       <c r="M420">
         <v>649.42527694666</v>
       </c>
+      <c r="N420">
+        <v>33.03788111999833</v>
+      </c>
     </row>
     <row r="421" spans="1:14">
       <c r="A421" s="1" t="s">
@@ -5489,6 +5534,9 @@
       </c>
       <c r="M421">
         <v>546.0076576214276</v>
+      </c>
+      <c r="N421">
+        <v>27.43742125943521</v>
       </c>
     </row>
     <row r="422" spans="1:14">

</xml_diff>